<commit_message>
LSTM with weather forecast
</commit_message>
<xml_diff>
--- a/model_comparison.xlsx
+++ b/model_comparison.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\shmiggit\code\AmaurySalles\projectwind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1156E29A-E2A4-414E-936F-DC17B2A0B93B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A148E7F-E033-43E6-84F5-27A6D98BBDEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{662292D5-D2C5-4A6D-89A7-C4306D43B4BE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Neurons" sheetId="2" r:id="rId1"/>
+    <sheet name="Layers" sheetId="3" r:id="rId2"/>
+    <sheet name="Dropouts" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="17">
   <si>
     <t>Models</t>
   </si>
@@ -72,12 +74,27 @@
   <si>
     <t>Epoch</t>
   </si>
+  <si>
+    <t>3x0.3</t>
+  </si>
+  <si>
+    <t>2x0.2</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>3x0.1</t>
+  </si>
+  <si>
+    <t>3x0.2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,6 +109,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -114,14 +136,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -146,21 +174,21 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>83820</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>2743855</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:colOff>2895600</xdr:colOff>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>1754676</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4FA68F0-F1ED-48D9-9950-AD85FCF665C4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE9E1A99-830A-41F9-8877-31086190B8AB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -176,8 +204,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7185660" y="396240"/>
-          <a:ext cx="2660035" cy="1724196"/>
+          <a:off x="6560820" y="4038600"/>
+          <a:ext cx="2811780" cy="1724196"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -189,22 +217,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>26214</xdr:rowOff>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>102414</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>4122420</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>1722120</xdr:rowOff>
+      <xdr:colOff>4130040</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1798320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21B3A217-4EA8-4F87-9F78-3D6F9224C9A6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CAF2FE5-B598-445C-B38C-5C97836C1E97}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -227,8 +255,1204 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="10073640" y="391974"/>
+          <a:off x="9456420" y="4110534"/>
           <a:ext cx="4114800" cy="1695906"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>47651</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>2895599</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CBF6E09-859A-4D5A-8673-FCF711B8153C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6524651" y="5836920"/>
+          <a:ext cx="2847948" cy="1889760"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>4130040</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1714500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFAB3CA1-418E-41B1-A74C-FE31DF6A98F8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9517379" y="7711440"/>
+          <a:ext cx="4053841" cy="1653540"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>2948940</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>120136</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>4152900</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1813560</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D2405A2-5E4C-444D-AAC7-4BABF7354F78}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9425940" y="2307076"/>
+          <a:ext cx="4168140" cy="1693424"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>98308</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>2865120</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1805940</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAFC88EA-B7A3-45D8-884F-17D4A9447ECF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6575308" y="2263140"/>
+          <a:ext cx="2766812" cy="1729740"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>87146</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>2872740</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1783080</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6012F006-2657-49DC-9C1A-9A97FE166D8C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6564146" y="5920740"/>
+          <a:ext cx="2785594" cy="1691640"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>110341</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>4130040</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1798319</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{196D7312-2AA0-4118-8C2B-927E0A428E55}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9448800" y="5939641"/>
+          <a:ext cx="4122420" cy="1687978"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>137160</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>18800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>2910840</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6A3825F-57F5-4E27-A811-7351C02B1075}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6614160" y="384560"/>
+          <a:ext cx="2773680" cy="1840479"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>91986</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>4114800</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1760219</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFA32752-19CE-455F-BA97-32253A2DB390}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9494520" y="457746"/>
+          <a:ext cx="4061460" cy="1668233"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>2895600</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1754676</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE4760BA-98ED-46B1-BBA2-6E60016B6B0B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6560820" y="4038600"/>
+          <a:ext cx="2811780" cy="1724196"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>102414</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>4130040</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1798320</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21305DAD-4FD8-48FF-AB7B-D752B6FEA994}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9456420" y="4110534"/>
+          <a:ext cx="4114800" cy="1695906"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>47651</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>2895599</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B96D8E56-9137-4713-8CFE-670C782FD83C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6524651" y="5836920"/>
+          <a:ext cx="2847948" cy="1889760"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>4033872</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1714500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{234BCE77-D5DA-40EE-9AE2-BB8EF510A75C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9517379" y="5890260"/>
+          <a:ext cx="3957673" cy="1653540"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>2948940</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>120136</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>4152900</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1813560</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9E4BB82-EB79-411D-A256-2989F2125170}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9425940" y="2307076"/>
+          <a:ext cx="4168140" cy="1693424"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>98308</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>2865120</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1805940</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16017549-1BE4-45E8-83DA-26503ED1F741}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6575308" y="2263140"/>
+          <a:ext cx="2766812" cy="1729740"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>2895600</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1754676</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4FA68F0-F1ED-48D9-9950-AD85FCF665C4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6560820" y="4038600"/>
+          <a:ext cx="2811780" cy="1724196"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>102414</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>4130040</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1798320</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21B3A217-4EA8-4F87-9F78-3D6F9224C9A6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9456420" y="2289354"/>
+          <a:ext cx="4114800" cy="1695906"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>47651</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>2895599</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{237F22EE-EE4E-4D0E-BC1C-EAB1F3661CC5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6524651" y="4015740"/>
+          <a:ext cx="2847948" cy="1889760"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>4033872</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1714500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C98C8ECF-9EE8-48FF-9BEC-0C7A61D261E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9517379" y="4069080"/>
+          <a:ext cx="3957673" cy="1653540"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>2948940</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>120136</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>4152900</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1813560</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DDA4B92-02C7-42E1-92FB-2C957402E0BE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9425940" y="2307076"/>
+          <a:ext cx="4168140" cy="1693424"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>98308</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>2865120</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1805940</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75F7BE61-9F01-433A-9F28-735BCB1C563C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6575308" y="2263140"/>
+          <a:ext cx="2766812" cy="1729740"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -546,60 +1770,60 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{181DC8F0-0260-4335-BDDC-AF663614CEC9}">
-  <dimension ref="B2:N9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D516D8AE-4F6F-4B4A-B6B3-1B4E29B81092}">
+  <dimension ref="B2:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
+    <col min="1" max="1" width="1.88671875" customWidth="1"/>
     <col min="2" max="2" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="4" customWidth="1"/>
+    <col min="6" max="6" width="1.88671875" customWidth="1"/>
     <col min="7" max="10" width="10.44140625" customWidth="1"/>
     <col min="11" max="11" width="1.88671875" customWidth="1"/>
     <col min="13" max="13" width="43.21875" customWidth="1"/>
     <col min="14" max="14" width="61" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="2:14">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:14" s="1" customFormat="1" ht="143.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:14" s="1" customFormat="1" ht="143.4" customHeight="1">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -609,27 +1833,28 @@
       <c r="D3" s="1">
         <v>256</v>
       </c>
-      <c r="E3" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="G3" s="1">
-        <v>317.9153</v>
-      </c>
-      <c r="H3" s="1">
-        <v>318.41359999999997</v>
-      </c>
-      <c r="I3" s="1">
-        <v>418.72070000000002</v>
-      </c>
-      <c r="J3" s="1">
-        <v>419.22030000000001</v>
+      <c r="E3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="2">
+        <v>486.98270000000002</v>
+      </c>
+      <c r="H3" s="2">
+        <v>487.48169999999999</v>
+      </c>
+      <c r="I3" s="2">
+        <v>496.2072</v>
+      </c>
+      <c r="J3" s="2">
+        <v>496.70670000000001</v>
       </c>
       <c r="L3" s="1">
-        <v>116</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="M3"/>
       <c r="N3"/>
     </row>
-    <row r="4" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:14" s="1" customFormat="1" ht="143.4" customHeight="1">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -639,15 +1864,470 @@
       <c r="D4" s="1">
         <v>256</v>
       </c>
-      <c r="E4" s="1">
-        <v>0.3</v>
-      </c>
+      <c r="E4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="1">
+        <v>317.9153</v>
+      </c>
+      <c r="H4" s="1">
+        <v>318.41359999999997</v>
+      </c>
+      <c r="I4" s="1">
+        <v>418.72070000000002</v>
+      </c>
+      <c r="J4" s="1">
+        <v>419.22030000000001</v>
+      </c>
+      <c r="L4" s="1">
+        <v>116</v>
+      </c>
+      <c r="N4"/>
     </row>
-    <row r="5" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:14" s="1" customFormat="1" ht="143.4" customHeight="1">
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1">
+        <v>256</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="2">
+        <v>645.46019999999999</v>
+      </c>
+      <c r="H5" s="2">
+        <v>645.96010000000001</v>
+      </c>
+      <c r="I5" s="2">
+        <v>617.81320000000005</v>
+      </c>
+      <c r="J5" s="2">
+        <v>618.31320000000005</v>
+      </c>
+      <c r="L5" s="1">
+        <v>56</v>
+      </c>
+      <c r="M5"/>
+      <c r="N5"/>
+    </row>
+    <row r="6" spans="2:14" s="1" customFormat="1" ht="143.4" customHeight="1">
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1">
+        <v>256</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="2">
+        <v>323.90940000000001</v>
+      </c>
+      <c r="H6" s="2">
+        <v>324.4074</v>
+      </c>
+      <c r="I6" s="2">
+        <v>446.41680000000002</v>
+      </c>
+      <c r="J6" s="2">
+        <v>446.9162</v>
+      </c>
+      <c r="L6" s="1">
+        <v>111</v>
+      </c>
+      <c r="M6"/>
+      <c r="N6"/>
+    </row>
+    <row r="7" spans="2:14" s="1" customFormat="1" ht="143.4" customHeight="1">
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1">
+        <v>256</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="2">
+        <v>322.16550000000001</v>
+      </c>
+      <c r="H7" s="2">
+        <v>322.6644</v>
+      </c>
+      <c r="I7" s="2">
+        <v>440.24369999999999</v>
+      </c>
+      <c r="J7" s="2">
+        <v>440.74329999999998</v>
+      </c>
+      <c r="L7" s="1">
+        <v>130</v>
+      </c>
+      <c r="M7"/>
+      <c r="N7"/>
+    </row>
+    <row r="8" spans="2:14" s="1" customFormat="1"/>
+    <row r="9" spans="2:14" s="1" customFormat="1"/>
+    <row r="10" spans="2:14" s="1" customFormat="1"/>
+    <row r="11" spans="2:14" s="1" customFormat="1"/>
+    <row r="12" spans="2:14" s="1" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6876622-E52D-4AB6-9455-DC40AC39EC15}">
+  <dimension ref="B2:N11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="1.88671875" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" customWidth="1"/>
+    <col min="6" max="6" width="1.88671875" customWidth="1"/>
+    <col min="7" max="10" width="10.44140625" customWidth="1"/>
+    <col min="11" max="11" width="1.88671875" customWidth="1"/>
+    <col min="13" max="13" width="43.21875" customWidth="1"/>
+    <col min="14" max="14" width="61" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:14">
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" s="1" customFormat="1" ht="143.4" customHeight="1">
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1">
+        <v>256</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3"/>
+    </row>
+    <row r="4" spans="2:14" s="1" customFormat="1" ht="143.4" customHeight="1">
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1">
+        <v>256</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="2">
+        <v>645.46019999999999</v>
+      </c>
+      <c r="H4" s="2">
+        <v>645.96010000000001</v>
+      </c>
+      <c r="I4" s="2">
+        <v>617.81320000000005</v>
+      </c>
+      <c r="J4" s="2">
+        <v>618.31320000000005</v>
+      </c>
+      <c r="L4" s="1">
+        <v>56</v>
+      </c>
+      <c r="M4"/>
+      <c r="N4"/>
+    </row>
+    <row r="5" spans="2:14" s="1" customFormat="1" ht="143.4" customHeight="1">
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1">
+        <v>256</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="1">
+        <v>317.9153</v>
+      </c>
+      <c r="H5" s="1">
+        <v>318.41359999999997</v>
+      </c>
+      <c r="I5" s="1">
+        <v>418.72070000000002</v>
+      </c>
+      <c r="J5" s="1">
+        <v>419.22030000000001</v>
+      </c>
+      <c r="L5" s="1">
+        <v>116</v>
+      </c>
+      <c r="N5"/>
+    </row>
+    <row r="6" spans="2:14" s="1" customFormat="1" ht="143.4" customHeight="1">
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1">
+        <v>256</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="2">
+        <v>322.16550000000001</v>
+      </c>
+      <c r="H6" s="2">
+        <v>322.6644</v>
+      </c>
+      <c r="I6" s="2">
+        <v>440.24369999999999</v>
+      </c>
+      <c r="J6" s="2">
+        <v>440.74329999999998</v>
+      </c>
+      <c r="L6" s="1">
+        <v>130</v>
+      </c>
+      <c r="M6"/>
+      <c r="N6"/>
+    </row>
+    <row r="7" spans="2:14" s="1" customFormat="1"/>
+    <row r="8" spans="2:14" s="1" customFormat="1"/>
+    <row r="9" spans="2:14" s="1" customFormat="1"/>
+    <row r="10" spans="2:14" s="1" customFormat="1"/>
+    <row r="11" spans="2:14" s="1" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{181DC8F0-0260-4335-BDDC-AF663614CEC9}">
+  <dimension ref="B2:N11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="1.88671875" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" customWidth="1"/>
+    <col min="6" max="6" width="1.88671875" customWidth="1"/>
+    <col min="7" max="10" width="10.44140625" customWidth="1"/>
+    <col min="11" max="11" width="1.88671875" customWidth="1"/>
+    <col min="13" max="13" width="43.21875" customWidth="1"/>
+    <col min="14" max="14" width="61" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:14">
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" s="1" customFormat="1" ht="143.4" customHeight="1">
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1">
+        <v>256</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3"/>
+    </row>
+    <row r="4" spans="2:14" s="1" customFormat="1" ht="143.4" customHeight="1">
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1">
+        <v>256</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="2">
+        <v>645.46019999999999</v>
+      </c>
+      <c r="H4" s="2">
+        <v>645.96010000000001</v>
+      </c>
+      <c r="I4" s="2">
+        <v>617.81320000000005</v>
+      </c>
+      <c r="J4" s="2">
+        <v>618.31320000000005</v>
+      </c>
+      <c r="L4" s="1">
+        <v>56</v>
+      </c>
+      <c r="M4"/>
+      <c r="N4"/>
+    </row>
+    <row r="5" spans="2:14" s="1" customFormat="1" ht="143.4" customHeight="1">
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1">
+        <v>256</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="1">
+        <v>317.9153</v>
+      </c>
+      <c r="H5" s="1">
+        <v>318.41359999999997</v>
+      </c>
+      <c r="I5" s="1">
+        <v>418.72070000000002</v>
+      </c>
+      <c r="J5" s="1">
+        <v>419.22030000000001</v>
+      </c>
+      <c r="L5" s="1">
+        <v>116</v>
+      </c>
+      <c r="N5"/>
+    </row>
+    <row r="6" spans="2:14" s="1" customFormat="1" ht="143.4" customHeight="1">
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1">
+        <v>256</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="2">
+        <v>322.16550000000001</v>
+      </c>
+      <c r="H6" s="2">
+        <v>322.6644</v>
+      </c>
+      <c r="I6" s="2">
+        <v>440.24369999999999</v>
+      </c>
+      <c r="J6" s="2">
+        <v>440.74329999999998</v>
+      </c>
+      <c r="L6" s="1">
+        <v>130</v>
+      </c>
+      <c r="M6"/>
+      <c r="N6"/>
+    </row>
+    <row r="7" spans="2:14" s="1" customFormat="1"/>
+    <row r="8" spans="2:14" s="1" customFormat="1"/>
+    <row r="9" spans="2:14" s="1" customFormat="1"/>
+    <row r="10" spans="2:14" s="1" customFormat="1"/>
+    <row r="11" spans="2:14" s="1" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Minor update to make window forecast optional
</commit_message>
<xml_diff>
--- a/model_comparison.xlsx
+++ b/model_comparison.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\shmiggit\code\AmaurySalles\projectwind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F12F69D-B058-4CDE-A5EE-5940FA9E633B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D7F3D54-9313-44C3-B03D-50B1DBDA42D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{662292D5-D2C5-4A6D-89A7-C4306D43B4BE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{662292D5-D2C5-4A6D-89A7-C4306D43B4BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Data &amp; Model" sheetId="7" r:id="rId1"/>
     <sheet name="Numerical" sheetId="6" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="10" r:id="rId3"/>
+    <sheet name="Weather Forecast" sheetId="11" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="83">
   <si>
     <t>LSTM</t>
   </si>
@@ -317,6 +319,50 @@
   </si>
   <si>
     <t>Weather Fcast</t>
+  </si>
+  <si>
+    <t>1x0.2</t>
+  </si>
+  <si>
+    <t>1X32LSTM
+2x64D</t>
+  </si>
+  <si>
+    <t>3x64LSTM</t>
+  </si>
+  <si>
+    <t>1x144
+1x72
+1x12</t>
+  </si>
+  <si>
+    <t>1x64D</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1X32LSTM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2x128D</t>
+    </r>
+  </si>
+  <si>
+    <t>1X64LSTM
+2x64D</t>
   </si>
 </sst>
 </file>
@@ -1325,7 +1371,49 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1518,7 +1606,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="12795266" y="2491740"/>
+          <a:off x="12894326" y="2491740"/>
           <a:ext cx="2749534" cy="1617820"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1784,16 +1872,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>117626</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>83820</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>2842260</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>1775460</xdr:rowOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>50918</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1823,8 +1911,501 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="12919226" y="6118860"/>
-          <a:ext cx="2724634" cy="1691640"/>
+          <a:off x="4221480" y="6118860"/>
+          <a:ext cx="11422380" cy="7091798"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>109147</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>2842259</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5261CAE-4533-42CC-AF4E-7B73D236BAB9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12910747" y="632460"/>
+          <a:ext cx="2733112" cy="1813560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>127743</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>4093538</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1798320</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0010568E-00C2-4B96-9015-F7ADCE58E56C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8745963" y="640080"/>
+          <a:ext cx="3965795" cy="1729740"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>25942</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>4122420</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1790700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DC103CD-9FA1-4225-B686-DEC9B9B4F431}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8686800" y="2418622"/>
+          <a:ext cx="4053840" cy="1764758"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>91439</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>109528</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>2857500</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1798319</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED3EEC51-E41E-4AFC-AF31-FAA44F2C53EA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12893039" y="2502208"/>
+          <a:ext cx="2766061" cy="1688791"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>6476</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>4137660</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1760220</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3D9D75A-33E3-469B-86BB-D5D164566531}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8618220" y="4220336"/>
+          <a:ext cx="4137660" cy="1753744"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>101634</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>2849879</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5F3ED33-AE69-49B5-B435-2FB6B79B0833}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12903234" y="4259580"/>
+          <a:ext cx="2748245" cy="1798320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>86734</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>2834640</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1798320</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD32BA07-51EA-4B3B-B936-0B7CA18B5D4B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12888334" y="6103620"/>
+          <a:ext cx="2747906" cy="1729740"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1564</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>4122420</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1783080</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{059CD8BA-8AFB-436B-B3BA-BC6D291D21DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8663940" y="6036604"/>
+          <a:ext cx="4076700" cy="1781516"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2145,7 +2726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2804C43-F2FA-40C8-82E5-2AEF3D65D292}">
   <dimension ref="B2:S57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+    <sheetView topLeftCell="A38" workbookViewId="0">
       <selection activeCell="M45" sqref="M45"/>
     </sheetView>
   </sheetViews>
@@ -2752,8 +3333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEDD5F94-9E14-4DC4-A0DA-5A6669DB9C70}">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView topLeftCell="F6" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3124,6 +3705,640 @@
     <mergeCell ref="I2:N2"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+      <formula>"S"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52876908-678B-4D94-8A35-6BA82775DAE4}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C8E1B3D-154F-4486-84C7-26B42CDD2CB0}">
+  <dimension ref="A1:Q22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="1.88671875" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10" style="53" customWidth="1"/>
+    <col min="4" max="4" width="8.77734375" style="53" customWidth="1"/>
+    <col min="5" max="5" width="10.21875" style="53" customWidth="1"/>
+    <col min="6" max="6" width="8" style="53" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" style="53" customWidth="1"/>
+    <col min="8" max="8" width="8.21875" style="53" customWidth="1"/>
+    <col min="9" max="14" width="9" style="53" customWidth="1"/>
+    <col min="15" max="15" width="6.21875" style="53" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="61" customWidth="1"/>
+    <col min="17" max="17" width="43.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="15" thickBot="1"/>
+    <row r="2" spans="1:17" ht="15" thickBot="1">
+      <c r="C2" s="57" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="58"/>
+      <c r="E2" s="61" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="62"/>
+      <c r="G2" s="71" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="72"/>
+      <c r="I2" s="66" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="68"/>
+    </row>
+    <row r="3" spans="1:17" ht="15" thickBot="1">
+      <c r="B3" s="69" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="60" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="60" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="60" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="64" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="65" t="s">
+        <v>6</v>
+      </c>
+      <c r="M3" s="64" t="s">
+        <v>4</v>
+      </c>
+      <c r="N3" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="O3" s="70" t="s">
+        <v>9</v>
+      </c>
+      <c r="P3" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q3" s="56" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" s="1" customFormat="1" ht="143.4" customHeight="1">
+      <c r="A4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="77" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="75" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="54" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" s="2">
+        <v>3.7900000000000003E-2</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0.15440000000000001</v>
+      </c>
+      <c r="K4" s="2">
+        <v>4.8399999999999999E-2</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0.17460000000000001</v>
+      </c>
+      <c r="M4" s="2">
+        <v>5.1400000000000001E-2</v>
+      </c>
+      <c r="N4" s="2">
+        <v>0.19070000000000001</v>
+      </c>
+      <c r="O4" s="54">
+        <v>146</v>
+      </c>
+      <c r="P4"/>
+      <c r="Q4"/>
+    </row>
+    <row r="5" spans="1:17" s="1" customFormat="1" ht="143.4" customHeight="1">
+      <c r="A5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="77" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="77" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="54" t="s">
+        <v>76</v>
+      </c>
+      <c r="G5" s="76" t="s">
+        <v>77</v>
+      </c>
+      <c r="H5" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" s="2">
+        <v>3.4200000000000001E-2</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0.14510000000000001</v>
+      </c>
+      <c r="K5" s="2">
+        <v>4.8500000000000001E-2</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0.1734</v>
+      </c>
+      <c r="M5" s="2">
+        <v>4.8599999999999997E-2</v>
+      </c>
+      <c r="N5" s="2">
+        <v>0.18360000000000001</v>
+      </c>
+      <c r="O5" s="54">
+        <v>62</v>
+      </c>
+      <c r="P5"/>
+      <c r="Q5"/>
+    </row>
+    <row r="6" spans="1:17" s="1" customFormat="1" ht="143.4" customHeight="1">
+      <c r="A6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="77" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="77" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="55" t="s">
+        <v>79</v>
+      </c>
+      <c r="F6" s="54" t="s">
+        <v>76</v>
+      </c>
+      <c r="G6" s="55" t="s">
+        <v>80</v>
+      </c>
+      <c r="H6" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="I6" s="2">
+        <v>2.9399999999999999E-2</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.1331</v>
+      </c>
+      <c r="K6" s="2">
+        <v>4.6399999999999997E-2</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0.17219999999999999</v>
+      </c>
+      <c r="M6" s="2">
+        <v>5.0299999999999997E-2</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0.1888</v>
+      </c>
+      <c r="O6" s="54">
+        <v>55</v>
+      </c>
+      <c r="P6"/>
+      <c r="Q6"/>
+    </row>
+    <row r="7" spans="1:17" s="1" customFormat="1" ht="143.4" customHeight="1">
+      <c r="A7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="77" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="77" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="54" t="s">
+        <v>76</v>
+      </c>
+      <c r="G7" s="76" t="s">
+        <v>81</v>
+      </c>
+      <c r="H7" s="75" t="s">
+        <v>76</v>
+      </c>
+      <c r="I7" s="2">
+        <v>3.1300000000000001E-2</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0.13739999999999999</v>
+      </c>
+      <c r="K7" s="2">
+        <v>4.6600000000000003E-2</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0.17369999999999999</v>
+      </c>
+      <c r="M7" s="2">
+        <v>5.0200000000000002E-2</v>
+      </c>
+      <c r="N7" s="2">
+        <v>0.18479999999999999</v>
+      </c>
+      <c r="O7" s="54">
+        <v>63</v>
+      </c>
+      <c r="P7"/>
+      <c r="Q7"/>
+    </row>
+    <row r="8" spans="1:17" s="1" customFormat="1" ht="143.4" customHeight="1">
+      <c r="A8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="77" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="77" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="54" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" s="76" t="s">
+        <v>82</v>
+      </c>
+      <c r="H8" s="77" t="s">
+        <v>76</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="54"/>
+      <c r="P8"/>
+      <c r="Q8"/>
+    </row>
+    <row r="9" spans="1:17" s="1" customFormat="1" ht="143.4" customHeight="1">
+      <c r="A9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="77"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="54"/>
+      <c r="P9"/>
+      <c r="Q9"/>
+    </row>
+    <row r="10" spans="1:17" s="1" customFormat="1" ht="143.4" customHeight="1">
+      <c r="A10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="54"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+    </row>
+    <row r="11" spans="1:17" s="1" customFormat="1" ht="143.4" customHeight="1">
+      <c r="A11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="77"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="55"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="54"/>
+      <c r="P11"/>
+      <c r="Q11"/>
+    </row>
+    <row r="12" spans="1:17" s="1" customFormat="1" ht="143.4" customHeight="1">
+      <c r="A12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="77"/>
+      <c r="D12" s="75"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="55"/>
+      <c r="H12" s="54"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="54"/>
+      <c r="P12"/>
+      <c r="Q12"/>
+    </row>
+    <row r="13" spans="1:17" s="1" customFormat="1" ht="143.4" customHeight="1">
+      <c r="A13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="77"/>
+      <c r="D13" s="75"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="55"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="54"/>
+      <c r="P13"/>
+      <c r="Q13"/>
+    </row>
+    <row r="14" spans="1:17" s="1" customFormat="1" ht="143.4" customHeight="1">
+      <c r="A14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="77"/>
+      <c r="D14" s="75"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="54"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="54"/>
+      <c r="P14"/>
+      <c r="Q14"/>
+    </row>
+    <row r="15" spans="1:17" s="1" customFormat="1" ht="143.4" customHeight="1">
+      <c r="A15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="77"/>
+      <c r="D15" s="75"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="54"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="54"/>
+      <c r="P15"/>
+      <c r="Q15"/>
+    </row>
+    <row r="16" spans="1:17" s="1" customFormat="1" ht="143.4" customHeight="1">
+      <c r="A16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="77"/>
+      <c r="D16" s="75"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="55"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="54"/>
+      <c r="P16"/>
+      <c r="Q16"/>
+    </row>
+    <row r="17" spans="1:17" s="1" customFormat="1" ht="143.4" customHeight="1">
+      <c r="A17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="77"/>
+      <c r="D17" s="75"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="55"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="54"/>
+      <c r="P17"/>
+      <c r="Q17"/>
+    </row>
+    <row r="18" spans="1:17" s="1" customFormat="1">
+      <c r="C18" s="77"/>
+      <c r="D18" s="75"/>
+      <c r="E18" s="55"/>
+      <c r="F18" s="54"/>
+      <c r="G18" s="55"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="54"/>
+      <c r="J18" s="54"/>
+      <c r="K18" s="54"/>
+      <c r="L18" s="54"/>
+      <c r="M18" s="54"/>
+      <c r="N18" s="54"/>
+      <c r="O18" s="54"/>
+    </row>
+    <row r="19" spans="1:17" s="1" customFormat="1">
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="54"/>
+      <c r="K19" s="54"/>
+      <c r="L19" s="54"/>
+      <c r="M19" s="54"/>
+      <c r="N19" s="54"/>
+      <c r="O19" s="54"/>
+    </row>
+    <row r="20" spans="1:17" s="1" customFormat="1">
+      <c r="C20" s="54"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="54"/>
+      <c r="F20" s="54"/>
+      <c r="G20" s="54"/>
+      <c r="H20" s="54"/>
+      <c r="I20" s="54"/>
+      <c r="J20" s="54"/>
+      <c r="K20" s="54"/>
+      <c r="L20" s="54"/>
+      <c r="M20" s="54"/>
+      <c r="N20" s="54"/>
+      <c r="O20" s="54"/>
+    </row>
+    <row r="21" spans="1:17" s="1" customFormat="1">
+      <c r="C21" s="54"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="54"/>
+      <c r="H21" s="54"/>
+      <c r="I21" s="54"/>
+      <c r="J21" s="54"/>
+      <c r="K21" s="54"/>
+      <c r="L21" s="54"/>
+      <c r="M21" s="54"/>
+      <c r="N21" s="54"/>
+      <c r="O21" s="54"/>
+    </row>
+    <row r="22" spans="1:17" s="1" customFormat="1">
+      <c r="C22" s="54"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="54"/>
+      <c r="F22" s="54"/>
+      <c r="G22" s="54"/>
+      <c r="H22" s="54"/>
+      <c r="I22" s="54"/>
+      <c r="J22" s="54"/>
+      <c r="K22" s="54"/>
+      <c r="L22" s="54"/>
+      <c r="M22" s="54"/>
+      <c r="N22" s="54"/>
+      <c r="O22" s="54"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:N2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A1:A4 A18:A1048576">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"S"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"S"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6:A17">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"S"</formula>
     </cfRule>

</xml_diff>